<commit_message>
Fix grammar and spelling
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Teaching\Students\CSharpDaniels\Bank Account\BankAccountStartProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B34C64-0448-4A00-A58E-B6B6927CA17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB5C7EA-B7FD-427F-B9C7-DB39925FB5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{231DA04D-6DAE-44B8-BAB9-18B26F92E78E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{231DA04D-6DAE-44B8-BAB9-18B26F92E78E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -123,18 +123,7 @@
 You must now store the bank accounts in a database so when the application starts up the old data is still present</t>
   </si>
   <si>
-    <t>-Setup database locally
-- Create a database project
-- Import database as C# classes into a db csproj
-- Create a new class that implements the IAccountRepository interface using entity framework
-- Remove Inmemory Account Repository class
-- When implementing the Updating Account - Ensure only the Balance, Withdrawn and PaidIn fields value change. Any other changes should be ingored</t>
-  </si>
-  <si>
     <t>Phase 3</t>
-  </si>
-  <si>
-    <t>In this phase the users have requested a nicer online user interface. A separate team will be building the online user interface but you task is to build a webservice with the endpoints for the operations they want to perform on the bank app.</t>
   </si>
   <si>
     <t>Account Service API</t>
@@ -173,12 +162,23 @@
     <t>(Extra) Email addresses</t>
   </si>
   <si>
-    <t>We've received reports that users are entering values that are not email addresses when creating an email. Enforce a check to make sure the email addresses are valid when creating an account</t>
+    <t>In this phase the users have requested a nicer online user interface. A separate team will be building the online user interface. Your task is to build a webservice with the endpoints for the operations they want to perform on the bank app.</t>
   </si>
   <si>
     <t>Ensure:
-- Email addresses contain an '@' and a '.'
-- Reject email address that fail this validation (throw exception) and don't create account</t>
+- Email addresses must contain '@' and '.'
+- Reject email address that fail this validation (throw exception) and don't create an account</t>
+  </si>
+  <si>
+    <t>We've received reports that users are entering values that are not vaild email addresses when creating an account. Enforce a check to make sure the email addresses are valid when creating an account</t>
+  </si>
+  <si>
+    <t>- Setup a database locally. You should store the accounts information in the database
+- Create a C# database project
+- Import database as C# classes into a db csproj
+- Create a new class that implements the IAccountRepository interface using entity framework
+- Remove InMemoryAccountRepository class and its tests (InMemoryAccountRepositoryTests)
+- When implementing the Updating Account - Ensure only the Balance, Withdrawn and PaidIn fields value change. Any other changes should be ingored</t>
   </si>
 </sst>
 </file>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55B2D190-E5AA-41D8-965F-759EB4428387}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -598,7 +598,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="116" x14ac:dyDescent="0.35">
@@ -637,7 +637,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>21</v>
@@ -648,13 +648,13 @@
         <v>1.6</v>
       </c>
       <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -682,7 +682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="145" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2.2000000000000002</v>
       </c>
@@ -693,7 +693,7 @@
         <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -702,7 +702,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -712,13 +712,13 @@
         <v>3.1</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -726,13 +726,13 @@
         <v>3.2</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>